<commit_message>
Updated the documents (updated Functional Tests and added System Documentation)
</commit_message>
<xml_diff>
--- a/Documents/Functional Tests - System administration module.xlsx
+++ b/Documents/Functional Tests - System administration module.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rtoir\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rtoir\Downloads\Testowanie Oprogramowania\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4881E622-0974-45A2-9B40-AEFF40F1FA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF35722A-3A7D-487D-B0B8-2FA964FEACE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FEBD750-072C-48FA-BE1C-244871805C24}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9FEBD750-072C-48FA-BE1C-244871805C24}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional Tests" sheetId="1" r:id="rId1"/>
@@ -264,7 +264,7 @@
     <t>The user remains logged in.</t>
   </si>
   <si>
-    <t>to be completed</t>
+    <t>17.03.2022</t>
   </si>
 </sst>
 </file>
@@ -274,7 +274,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,11 +315,16 @@
       <charset val="238"/>
     </font>
     <font>
-      <i/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -653,18 +658,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -742,6 +735,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1064,7 +1069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD05296-BF9F-4B70-8DBE-BB92CA27D7FD}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F3" sqref="F3:F5"/>
     </sheetView>
   </sheetViews>
@@ -1083,21 +1088,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="41" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="43"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="39"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="24.75" customHeight="1" thickBot="1">
@@ -1137,25 +1142,25 @@
       <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:12" ht="106.5" customHeight="1">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="46" t="s">
         <v>52</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -1173,13 +1178,13 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="106.5" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="51"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="47"/>
       <c r="H4" s="6" t="s">
         <v>37</v>
       </c>
@@ -1195,13 +1200,13 @@
       <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:12" ht="106.5" customHeight="1" thickBot="1">
-      <c r="A5" s="46"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="52"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="21" t="s">
         <v>38</v>
       </c>
@@ -1400,8 +1405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51B269C-A11B-41F2-B2B7-9B8EF1E55741}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1416,185 +1421,186 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" thickBot="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="71.25" customHeight="1">
-      <c r="A2" s="28">
+      <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="1:9" ht="71.25" customHeight="1">
-      <c r="A3" s="31">
+      <c r="A3" s="27">
         <v>2</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:9" ht="71.25" customHeight="1" thickBot="1">
-      <c r="A4" s="34">
+      <c r="A4" s="30">
         <v>3</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="36"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="32"/>
     </row>
     <row r="5" spans="1:9" ht="66" customHeight="1" thickBot="1">
-      <c r="A5" s="37">
+      <c r="A5" s="33">
         <v>4</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="40"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="36"/>
     </row>
     <row r="6" spans="1:9" ht="66" customHeight="1" thickBot="1">
-      <c r="A6" s="37">
+      <c r="A6" s="33">
         <v>5</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="40"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="36"/>
     </row>
     <row r="7" spans="1:9" ht="66" customHeight="1" thickBot="1">
-      <c r="A7" s="37">
+      <c r="A7" s="33">
         <v>6</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="38"/>
-      <c r="I7" s="40"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="36"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Merging project with new module: Business Administration
</commit_message>
<xml_diff>
--- a/Documents/Functional Tests - System administration module.xlsx
+++ b/Documents/Functional Tests - System administration module.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rtoir\Downloads\Testowanie Oprogramowania\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rtoir\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF35722A-3A7D-487D-B0B8-2FA964FEACE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4881E622-0974-45A2-9B40-AEFF40F1FA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9FEBD750-072C-48FA-BE1C-244871805C24}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FEBD750-072C-48FA-BE1C-244871805C24}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional Tests" sheetId="1" r:id="rId1"/>
@@ -264,7 +264,7 @@
     <t>The user remains logged in.</t>
   </si>
   <si>
-    <t>17.03.2022</t>
+    <t>to be completed</t>
   </si>
 </sst>
 </file>
@@ -274,7 +274,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,16 +315,11 @@
       <charset val="238"/>
     </font>
     <font>
+      <i/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -658,6 +653,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -735,18 +742,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1069,7 +1064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD05296-BF9F-4B70-8DBE-BB92CA27D7FD}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F3" sqref="F3:F5"/>
     </sheetView>
   </sheetViews>
@@ -1088,21 +1083,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="37" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="39"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="43"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="24.75" customHeight="1" thickBot="1">
@@ -1142,25 +1137,25 @@
       <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:12" ht="106.5" customHeight="1">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="50" t="s">
         <v>52</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -1178,13 +1173,13 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="106.5" customHeight="1">
-      <c r="A4" s="41"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="47"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="6" t="s">
         <v>37</v>
       </c>
@@ -1200,13 +1195,13 @@
       <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:12" ht="106.5" customHeight="1" thickBot="1">
-      <c r="A5" s="42"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="48"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="21" t="s">
         <v>38</v>
       </c>
@@ -1405,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51B269C-A11B-41F2-B2B7-9B8EF1E55741}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1421,186 +1416,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" thickBot="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="27" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="71.25" customHeight="1">
-      <c r="A2" s="24">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="71.25" customHeight="1">
-      <c r="A3" s="27">
+      <c r="A3" s="31">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="29"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:9" ht="71.25" customHeight="1" thickBot="1">
-      <c r="A4" s="30">
+      <c r="A4" s="34">
         <v>3</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="31"/>
-      <c r="I4" s="32"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
     </row>
     <row r="5" spans="1:9" ht="66" customHeight="1" thickBot="1">
-      <c r="A5" s="33">
+      <c r="A5" s="37">
         <v>4</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="H5" s="34"/>
-      <c r="I5" s="36"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="40"/>
     </row>
     <row r="6" spans="1:9" ht="66" customHeight="1" thickBot="1">
-      <c r="A6" s="33">
+      <c r="A6" s="37">
         <v>5</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="34"/>
-      <c r="I6" s="36"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="40"/>
     </row>
     <row r="7" spans="1:9" ht="66" customHeight="1" thickBot="1">
-      <c r="A7" s="33">
+      <c r="A7" s="37">
         <v>6</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="34"/>
-      <c r="I7" s="36"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="40"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>